<commit_message>
add code to write back into excel
</commit_message>
<xml_diff>
--- a/resource/Questionare on Regression testing.xlsx
+++ b/resource/Questionare on Regression testing.xlsx
@@ -4,7 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="LogError" sheetId="2" r:id="rId2"/>
+    <sheet name="StatusSheet77618" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -377,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA1048576"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -400,9 +400,6 @@
       </c>
       <c r="F1" t="str">
         <v>Level</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Status</v>
       </c>
     </row>
     <row r="2">
@@ -779,7 +776,7 @@
   </hyperlinks>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AA1048576"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F21"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>